<commit_message>
STM32G benchmark and tabs / optimization model for stm32g
</commit_message>
<xml_diff>
--- a/graphs/STM32G/dijkstra/dijkstra.xlsx
+++ b/graphs/STM32G/dijkstra/dijkstra.xlsx
@@ -6,11 +6,12 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="data_RAM NORMAL" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="data_RAM CODE_CCM" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet name="data_RAM CACHE_OFF_PRE_OFF" sheetId="3" state="visible" r:id="rId3"/>
-    <sheet name="data_RAM CACHE_OFF_PRE_ON" sheetId="4" state="visible" r:id="rId4"/>
-    <sheet name="data_RAM CACHE_ON_PRE_ON" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet name="NORMAL" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="CODE_CCM" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="CODE_CCM-CACHE_OFF" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="CACHE_OFF-PRE_OFF" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet name="CACHE_OFF-PRE_ON" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet name="CACHE_ON-PRE_ON" sheetId="6" state="visible" r:id="rId6"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -463,261 +464,261 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="B1" s="2" t="inlineStr">
+      <c r="B1" s="1" t="inlineStr">
         <is>
           <t>16_RANGE2</t>
         </is>
       </c>
-      <c r="C1" s="2" t="inlineStr">
+      <c r="C1" s="1" t="inlineStr">
         <is>
           <t>26_RANGE2</t>
         </is>
       </c>
-      <c r="D1" s="2" t="inlineStr">
+      <c r="D1" s="1" t="inlineStr">
         <is>
           <t>16</t>
         </is>
       </c>
-      <c r="E1" s="2" t="inlineStr">
+      <c r="E1" s="1" t="inlineStr">
         <is>
           <t>26</t>
         </is>
       </c>
-      <c r="F1" s="2" t="inlineStr">
+      <c r="F1" s="1" t="inlineStr">
         <is>
           <t>30</t>
         </is>
       </c>
-      <c r="G1" s="2" t="inlineStr">
+      <c r="G1" s="1" t="inlineStr">
         <is>
           <t>60</t>
         </is>
       </c>
-      <c r="H1" s="2" t="inlineStr">
+      <c r="H1" s="1" t="inlineStr">
         <is>
           <t>90</t>
         </is>
       </c>
-      <c r="I1" s="2" t="inlineStr">
+      <c r="I1" s="1" t="inlineStr">
         <is>
           <t>120</t>
         </is>
       </c>
-      <c r="J1" s="2" t="inlineStr">
+      <c r="J1" s="1" t="inlineStr">
         <is>
           <t>150</t>
         </is>
       </c>
-      <c r="K1" s="2" t="inlineStr">
+      <c r="K1" s="1" t="inlineStr">
         <is>
           <t>170</t>
         </is>
       </c>
-      <c r="L1" s="2" t="inlineStr">
+      <c r="L1" s="1" t="inlineStr">
         <is>
           <t>150_BOOST</t>
         </is>
       </c>
-      <c r="M1" s="2" t="inlineStr">
+      <c r="M1" s="1" t="inlineStr">
         <is>
           <t>170_BOOST</t>
         </is>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="2" t="inlineStr">
+      <c r="A2" s="1" t="inlineStr">
         <is>
           <t>intensity</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>2764.620422678376</v>
+        <v>2774.966589163913</v>
       </c>
       <c r="C2" t="n">
-        <v>4189.577493169693</v>
+        <v>4152.742003361904</v>
       </c>
       <c r="D2" t="n">
-        <v>3275.422208784053</v>
+        <v>3290.354689077069</v>
       </c>
       <c r="E2" t="n">
-        <v>4980.268832211326</v>
+        <v>4985.146549401181</v>
       </c>
       <c r="F2" t="n">
-        <v>5668.593308705502</v>
+        <v>5666.441161276326</v>
       </c>
       <c r="G2" t="n">
-        <v>9992.116853788302</v>
+        <v>10020.94799004018</v>
       </c>
       <c r="H2" t="n">
-        <v>14678.63103138663</v>
+        <v>14523.23630452156</v>
       </c>
       <c r="I2" t="n">
-        <v>19171.79473502388</v>
+        <v>19117.25050802904</v>
       </c>
       <c r="J2" t="n">
-        <v>23907.30371715684</v>
+        <v>23715.64680690532</v>
       </c>
       <c r="K2" t="n">
-        <v>27080.02872264849</v>
+        <v>26762.71223416359</v>
       </c>
       <c r="L2" t="n">
-        <v>25682.13153195072</v>
+        <v>25400.98183852129</v>
       </c>
       <c r="M2" t="n">
-        <v>29032.09267414981</v>
+        <v>28733.768120228</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="2" t="inlineStr">
+      <c r="A3" s="1" t="inlineStr">
         <is>
           <t>runtime</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0.72058</v>
+        <v>0.7201</v>
       </c>
       <c r="C3" t="n">
-        <v>0.44398</v>
+        <v>0.4433</v>
       </c>
       <c r="D3" t="n">
-        <v>0.7208599999999999</v>
+        <v>0.72016</v>
       </c>
       <c r="E3" t="n">
-        <v>0.44366</v>
+        <v>0.4435</v>
       </c>
       <c r="F3" t="n">
-        <v>0.3845</v>
+        <v>0.38392</v>
       </c>
       <c r="G3" t="n">
-        <v>0.1925</v>
+        <v>0.1921</v>
       </c>
       <c r="H3" t="n">
-        <v>0.12808</v>
+        <v>0.128</v>
       </c>
       <c r="I3" t="n">
-        <v>0.09614</v>
+        <v>0.09606000000000001</v>
       </c>
       <c r="J3" t="n">
-        <v>0.07693999999999999</v>
+        <v>0.07674</v>
       </c>
       <c r="K3" t="n">
-        <v>0.06791999999999999</v>
+        <v>0.06772</v>
       </c>
       <c r="L3" t="n">
-        <v>0.077</v>
+        <v>0.07682</v>
       </c>
       <c r="M3" t="n">
-        <v>0.06794</v>
+        <v>0.06786</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="2" t="inlineStr">
+      <c r="A4" s="1" t="inlineStr">
         <is>
           <t>timestamp</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>(1838.14, 2558.72)</t>
+          <t>(1498.04, 2218.14)</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>(6241.28, 6685.26)</t>
+          <t>(6719.56, 7162.86)</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>(9446.56, 10167.42)</t>
+          <t>(10464.62, 11184.78)</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>(13850.8, 14294.46)</t>
+          <t>(15684.86, 16128.36)</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>(16867.8, 17252.3)</t>
+          <t>(19239.18, 19623.1)</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>(19586.46, 19778.96)</t>
+          <t>(22438.24, 22630.34)</t>
         </is>
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>(21344.62, 21472.7)</t>
+          <t>(24485.76, 24613.76)</t>
         </is>
       </c>
       <c r="I4" t="inlineStr">
         <is>
-          <t>(22835.96, 22932.1)</t>
+          <t>(26202.64, 26298.7)</t>
         </is>
       </c>
       <c r="J4" t="inlineStr">
         <is>
-          <t>(24154.36, 24231.3)</t>
+          <t>(27713.16, 27789.9)</t>
         </is>
       </c>
       <c r="K4" t="inlineStr">
         <is>
-          <t>(25398.24, 25466.16)</t>
+          <t>(29130.78, 29198.5)</t>
         </is>
       </c>
       <c r="L4" t="inlineStr">
         <is>
-          <t>(26589.32, 26666.32)</t>
+          <t>(30488.0, 30564.82)</t>
         </is>
       </c>
       <c r="M4" t="inlineStr">
         <is>
-          <t>(27832.02, 27899.96)</t>
+          <t>(31905.3, 31973.16)</t>
         </is>
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="2" t="inlineStr">
+      <c r="A5" s="1" t="inlineStr">
         <is>
           <t>energy</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>6574.029607772827</v>
+        <v>1998.253440856934</v>
       </c>
       <c r="C5" t="n">
-        <v>6138.292430877686</v>
+        <v>1840.910530090332</v>
       </c>
       <c r="D5" t="n">
-        <v>7791.698816299437</v>
+        <v>2843.498199462891</v>
       </c>
       <c r="E5" t="n">
-        <v>7291.502031326294</v>
+        <v>2653.094993591309</v>
       </c>
       <c r="F5" t="n">
-        <v>7192.594619750977</v>
+        <v>2610.552108764648</v>
       </c>
       <c r="G5" t="n">
-        <v>6347.492231369019</v>
+        <v>2310.028930664062</v>
       </c>
       <c r="H5" t="n">
-        <v>6204.128906249999</v>
+        <v>2230.769096374512</v>
       </c>
       <c r="I5" t="n">
-        <v>6082.481941223145</v>
+        <v>2203.683700561523</v>
       </c>
       <c r="J5" t="n">
-        <v>6070.112228393554</v>
+        <v>2183.926483154297</v>
       </c>
       <c r="K5" t="n">
-        <v>6069.609317779541</v>
+        <v>2174.84504699707</v>
       </c>
       <c r="L5" t="n">
-        <v>6525.829622268677</v>
+        <v>2497.668383789063</v>
       </c>
       <c r="M5" t="n">
-        <v>6509.053241729735</v>
+        <v>2495.8380859375</v>
       </c>
     </row>
   </sheetData>
@@ -808,40 +809,40 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>2567.641632161935</v>
+        <v>2567.412619704229</v>
       </c>
       <c r="C2" t="n">
-        <v>3870.68331592365</v>
+        <v>3849.958208939728</v>
       </c>
       <c r="D2" t="n">
-        <v>3052.471472537981</v>
+        <v>3064.70315165253</v>
       </c>
       <c r="E2" t="n">
-        <v>4618.581170346338</v>
+        <v>4604.188015135072</v>
       </c>
       <c r="F2" t="n">
-        <v>5254.637832036063</v>
+        <v>5231.769954302717</v>
       </c>
       <c r="G2" t="n">
-        <v>9189.068931336848</v>
+        <v>9106.526894849947</v>
       </c>
       <c r="H2" t="n">
-        <v>13470.63740514863</v>
+        <v>13311.31212026795</v>
       </c>
       <c r="I2" t="n">
-        <v>17757.24636101575</v>
+        <v>17539.8584959339</v>
       </c>
       <c r="J2" t="n">
-        <v>22025.65746005874</v>
+        <v>21735.43917179603</v>
       </c>
       <c r="K2" t="n">
-        <v>24886.59916909088</v>
+        <v>24549.45309077216</v>
       </c>
       <c r="L2" t="n">
-        <v>23674.24865975914</v>
+        <v>23408.13168360313</v>
       </c>
       <c r="M2" t="n">
-        <v>26722.36450114791</v>
+        <v>26419.53477570845</v>
       </c>
     </row>
     <row r="3">
@@ -851,40 +852,40 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0.72326</v>
+        <v>0.7228</v>
       </c>
       <c r="C3" t="n">
-        <v>0.44522</v>
+        <v>0.44468</v>
       </c>
       <c r="D3" t="n">
-        <v>0.72316</v>
+        <v>0.72278</v>
       </c>
       <c r="E3" t="n">
-        <v>0.44514</v>
+        <v>0.4448</v>
       </c>
       <c r="F3" t="n">
-        <v>0.38554</v>
+        <v>0.38542</v>
       </c>
       <c r="G3" t="n">
-        <v>0.19298</v>
+        <v>0.19274</v>
       </c>
       <c r="H3" t="n">
-        <v>0.12856</v>
+        <v>0.12838</v>
       </c>
       <c r="I3" t="n">
-        <v>0.09660000000000001</v>
+        <v>0.09622</v>
       </c>
       <c r="J3" t="n">
-        <v>0.07718</v>
+        <v>0.07704</v>
       </c>
       <c r="K3" t="n">
-        <v>0.06816</v>
+        <v>0.06794</v>
       </c>
       <c r="L3" t="n">
-        <v>0.07711999999999999</v>
+        <v>0.07704</v>
       </c>
       <c r="M3" t="n">
-        <v>0.06822</v>
+        <v>0.06806</v>
       </c>
     </row>
     <row r="4">
@@ -895,62 +896,62 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>(2658.38, 3381.64)</t>
+          <t>(2317.76, 3040.56)</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>(6784.98, 7230.2)</t>
+          <t>(7262.26, 7706.94)</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>(10266.74, 10989.9)</t>
+          <t>(11284.0, 12006.78)</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>(14394.2, 14839.34)</t>
+          <t>(16227.32, 16672.12)</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>(17351.66, 17737.2)</t>
+          <t>(19722.4, 20107.82)</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>(19878.76, 20071.74)</t>
+          <t>(22729.7, 22922.44)</t>
         </is>
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>(21572.42, 21700.98)</t>
+          <t>(24713.0, 24841.38)</t>
         </is>
       </c>
       <c r="I4" t="inlineStr">
         <is>
-          <t>(23031.66, 23128.26)</t>
+          <t>(26398.02, 26494.24)</t>
         </is>
       </c>
       <c r="J4" t="inlineStr">
         <is>
-          <t>(24331.04, 24408.22)</t>
+          <t>(27889.38, 27966.42)</t>
         </is>
       </c>
       <c r="K4" t="inlineStr">
         <is>
-          <t>(25565.78, 25633.94)</t>
+          <t>(29297.82, 29365.76)</t>
         </is>
       </c>
       <c r="L4" t="inlineStr">
         <is>
-          <t>(26765.98, 26843.1)</t>
+          <t>(30664.12, 30741.16)</t>
         </is>
       </c>
       <c r="M4" t="inlineStr">
         <is>
-          <t>(27999.44, 28067.66)</t>
+          <t>(32072.36, 32140.42)</t>
         </is>
       </c>
     </row>
@@ -961,40 +962,40 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>6128.339206695557</v>
+        <v>1855.725841522217</v>
       </c>
       <c r="C5" t="n">
-        <v>5686.90856552124</v>
+        <v>1711.999416351318</v>
       </c>
       <c r="D5" t="n">
-        <v>7284.50339126587</v>
+        <v>2658.127372741699</v>
       </c>
       <c r="E5" t="n">
-        <v>6784.520233154297</v>
+        <v>2457.531394958496</v>
       </c>
       <c r="F5" t="n">
-        <v>6685.381130218506</v>
+        <v>2419.714530944824</v>
       </c>
       <c r="G5" t="n">
-        <v>5851.91152381897</v>
+        <v>2106.230392456055</v>
       </c>
       <c r="H5" t="n">
-        <v>5714.890977859497</v>
+        <v>2050.6875</v>
       </c>
       <c r="I5" t="n">
-        <v>5660.6549949646</v>
+        <v>2025.222221374512</v>
       </c>
       <c r="J5" t="n">
-        <v>5609.802801132201</v>
+        <v>2009.397880554199</v>
       </c>
       <c r="K5" t="n">
-        <v>5597.692977905273</v>
+        <v>2001.467811584473</v>
       </c>
       <c r="L5" t="n">
-        <v>6025.001586914062</v>
+        <v>2308.303955078125</v>
       </c>
       <c r="M5" t="n">
-        <v>6015.899030685425</v>
+        <v>2301.585327148438</v>
       </c>
     </row>
   </sheetData>
@@ -1085,40 +1086,40 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>3266.471665061283</v>
+        <v>2568.583295469525</v>
       </c>
       <c r="C2" t="n">
-        <v>4412.31662404445</v>
+        <v>3850.098159290776</v>
       </c>
       <c r="D2" t="n">
-        <v>3942.333352437235</v>
+        <v>3065.456494690638</v>
       </c>
       <c r="E2" t="n">
-        <v>6023.586483936819</v>
+        <v>4606.126553671088</v>
       </c>
       <c r="F2" t="n">
-        <v>6852.582630567209</v>
+        <v>5233.509889644254</v>
       </c>
       <c r="G2" t="n">
-        <v>12259.81786769585</v>
+        <v>9105.849162241544</v>
       </c>
       <c r="H2" t="n">
-        <v>15519.5041356353</v>
+        <v>13317.5390760042</v>
       </c>
       <c r="I2" t="n">
-        <v>20373.47504841633</v>
+        <v>17533.91237383536</v>
       </c>
       <c r="J2" t="n">
-        <v>23543.48487504816</v>
+        <v>21735.23879415725</v>
       </c>
       <c r="K2" t="n">
-        <v>26548.21569636717</v>
+        <v>24551.1776487535</v>
       </c>
       <c r="L2" t="n">
-        <v>25363.99895630683</v>
+        <v>23421.38441154518</v>
       </c>
       <c r="M2" t="n">
-        <v>28586.57290221779</v>
+        <v>26427.09505190408</v>
       </c>
     </row>
     <row r="3">
@@ -1128,40 +1129,40 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0.72076</v>
+        <v>0.72244</v>
       </c>
       <c r="C3" t="n">
-        <v>0.54562</v>
+        <v>0.44438</v>
       </c>
       <c r="D3" t="n">
-        <v>0.72158</v>
+        <v>0.7226399999999999</v>
       </c>
       <c r="E3" t="n">
-        <v>0.44384</v>
+        <v>0.44454</v>
       </c>
       <c r="F3" t="n">
-        <v>0.38432</v>
+        <v>0.3852</v>
       </c>
       <c r="G3" t="n">
-        <v>0.1922</v>
+        <v>0.19292</v>
       </c>
       <c r="H3" t="n">
-        <v>0.1576</v>
+        <v>0.12836</v>
       </c>
       <c r="I3" t="n">
-        <v>0.11798</v>
+        <v>0.09642000000000001</v>
       </c>
       <c r="J3" t="n">
-        <v>0.10706</v>
+        <v>0.07718</v>
       </c>
       <c r="K3" t="n">
-        <v>0.0944</v>
+        <v>0.06802</v>
       </c>
       <c r="L3" t="n">
-        <v>0.10674</v>
+        <v>0.07718</v>
       </c>
       <c r="M3" t="n">
-        <v>0.09420000000000001</v>
+        <v>0.06809999999999999</v>
       </c>
     </row>
     <row r="4">
@@ -1172,62 +1173,62 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>(3481.42, 4202.18)</t>
+          <t>(3140.14, 3862.58)</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>(7329.96, 7875.58)</t>
+          <t>(7806.5, 8250.88)</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>(11089.66, 11811.24)</t>
+          <t>(12106.36, 12829.0)</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>(14939.14, 15382.98)</t>
+          <t>(16771.12, 17215.66)</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>(17836.52, 18220.84)</t>
+          <t>(20206.78, 20591.98)</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>(20171.16, 20363.36)</t>
+          <t>(23021.7, 23214.62)</t>
         </is>
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>(21800.44, 21958.04)</t>
+          <t>(24940.66, 25069.02)</t>
         </is>
       </c>
       <c r="I4" t="inlineStr">
         <is>
-          <t>(23227.8, 23345.78)</t>
+          <t>(26593.52, 26689.94)</t>
         </is>
       </c>
       <c r="J4" t="inlineStr">
         <is>
-          <t>(24507.92, 24614.98)</t>
+          <t>(28065.7, 28142.88)</t>
         </is>
       </c>
       <c r="K4" t="inlineStr">
         <is>
-          <t>(25733.32, 25827.72)</t>
+          <t>(29465.58, 29533.6)</t>
         </is>
       </c>
       <c r="L4" t="inlineStr">
         <is>
-          <t>(26942.56, 27049.3)</t>
+          <t>(30840.3, 30917.48)</t>
         </is>
       </c>
       <c r="M4" t="inlineStr">
         <is>
-          <t>(28167.52, 28261.72)</t>
+          <t>(32240.02, 32308.12)</t>
         </is>
       </c>
     </row>
@@ -1238,40 +1239,40 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>7769.328987121581</v>
+        <v>1855.647315979004</v>
       </c>
       <c r="C5" t="n">
-        <v>7944.579048156737</v>
+        <v>1710.906620025635</v>
       </c>
       <c r="D5" t="n">
-        <v>9387.539371490479</v>
+        <v>2658.265777587891</v>
       </c>
       <c r="E5" t="n">
-        <v>8822.578462600708</v>
+        <v>2457.128997802734</v>
       </c>
       <c r="F5" t="n">
-        <v>8690.829036712645</v>
+        <v>2419.13761138916</v>
       </c>
       <c r="G5" t="n">
-        <v>7775.912080764771</v>
+        <v>2108.040504455566</v>
       </c>
       <c r="H5" t="n">
-        <v>8071.383710861205</v>
+        <v>2051.327178955078</v>
       </c>
       <c r="I5" t="n">
-        <v>7932.086534500121</v>
+        <v>2028.743797302246</v>
       </c>
       <c r="J5" t="n">
-        <v>8317.866119384766</v>
+        <v>2013.030876159668</v>
       </c>
       <c r="K5" t="n">
-        <v>8270.300153732298</v>
+        <v>2003.965324401855</v>
       </c>
       <c r="L5" t="n">
-        <v>8934.265720367432</v>
+        <v>2313.807934570313</v>
       </c>
       <c r="M5" t="n">
-        <v>8886.422052383423</v>
+        <v>2303.597021484375</v>
       </c>
     </row>
   </sheetData>
@@ -1362,40 +1363,40 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>3313.392438799065</v>
+        <v>3269.826349418406</v>
       </c>
       <c r="C2" t="n">
-        <v>4593.851234745152</v>
+        <v>4406.160341800101</v>
       </c>
       <c r="D2" t="n">
-        <v>4017.374978673403</v>
+        <v>3965.819914952681</v>
       </c>
       <c r="E2" t="n">
-        <v>6091.265324994126</v>
+        <v>6010.189788965734</v>
       </c>
       <c r="F2" t="n">
-        <v>6921.214502893934</v>
+        <v>6818.530720621681</v>
       </c>
       <c r="G2" t="n">
-        <v>12349.87098840017</v>
+        <v>12175.33489623235</v>
       </c>
       <c r="H2" t="n">
-        <v>16061.47875418358</v>
+        <v>15354.21325613733</v>
       </c>
       <c r="I2" t="n">
-        <v>21053.57378799186</v>
+        <v>20151.61700136398</v>
       </c>
       <c r="J2" t="n">
-        <v>23303.27807600404</v>
+        <v>23271.19957763901</v>
       </c>
       <c r="K2" t="n">
-        <v>26279.67622589118</v>
+        <v>26244.83264462157</v>
       </c>
       <c r="L2" t="n">
-        <v>25113.6989768492</v>
+        <v>25118.03642741923</v>
       </c>
       <c r="M2" t="n">
-        <v>28303.66135832922</v>
+        <v>28289.26332587524</v>
       </c>
     </row>
     <row r="3">
@@ -1405,40 +1406,40 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0.72044</v>
+        <v>0.7198600000000001</v>
       </c>
       <c r="C3" t="n">
-        <v>0.52966</v>
+        <v>0.54478</v>
       </c>
       <c r="D3" t="n">
-        <v>0.72132</v>
+        <v>0.72082</v>
       </c>
       <c r="E3" t="n">
-        <v>0.4439</v>
+        <v>0.44314</v>
       </c>
       <c r="F3" t="n">
-        <v>0.38458</v>
+        <v>0.38394</v>
       </c>
       <c r="G3" t="n">
-        <v>0.19208</v>
+        <v>0.19192</v>
       </c>
       <c r="H3" t="n">
-        <v>0.15286</v>
+        <v>0.15726</v>
       </c>
       <c r="I3" t="n">
-        <v>0.1147</v>
+        <v>0.11802</v>
       </c>
       <c r="J3" t="n">
-        <v>0.1091</v>
+        <v>0.1067</v>
       </c>
       <c r="K3" t="n">
-        <v>0.09614</v>
+        <v>0.09418</v>
       </c>
       <c r="L3" t="n">
-        <v>0.109</v>
+        <v>0.10672</v>
       </c>
       <c r="M3" t="n">
-        <v>0.09622</v>
+        <v>0.09422</v>
       </c>
     </row>
     <row r="4">
@@ -1449,62 +1450,62 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>(4302.04, 5022.48)</t>
+          <t>(3962.22, 4682.08)</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>(7975.38, 8505.04)</t>
+          <t>(8350.36, 8895.14)</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>(11910.98, 12632.3)</t>
+          <t>(12928.32, 13649.14)</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>(15482.74, 15926.64)</t>
+          <t>(17314.72, 17757.86)</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>(18320.3, 18704.88)</t>
+          <t>(20691.34, 21075.28)</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>(20462.98, 20655.06)</t>
+          <t>(23313.8, 23505.72)</t>
         </is>
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>(22057.4, 22210.26)</t>
+          <t>(25168.54, 25325.8)</t>
         </is>
       </c>
       <c r="I4" t="inlineStr">
         <is>
-          <t>(23445.5, 23560.2)</t>
+          <t>(26789.1, 26907.12)</t>
         </is>
       </c>
       <c r="J4" t="inlineStr">
         <is>
-          <t>(24714.64, 24823.74)</t>
+          <t>(28242.02, 28348.72)</t>
         </is>
       </c>
       <c r="K4" t="inlineStr">
         <is>
-          <t>(25927.6, 26023.74)</t>
+          <t>(29633.04, 29727.22)</t>
         </is>
       </c>
       <c r="L4" t="inlineStr">
         <is>
-          <t>(27148.78, 27257.78)</t>
+          <t>(31017.22, 31123.94)</t>
         </is>
       </c>
       <c r="M4" t="inlineStr">
         <is>
-          <t>(28361.52, 28457.74)</t>
+          <t>(32407.48, 32501.7)</t>
         </is>
       </c>
     </row>
@@ -1515,40 +1516,40 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>7877.431480407715</v>
+        <v>2353.817195892334</v>
       </c>
       <c r="C5" t="n">
-        <v>8029.491508483888</v>
+        <v>2400.388031005859</v>
       </c>
       <c r="D5" t="n">
-        <v>9562.782634735107</v>
+        <v>3430.37077331543</v>
       </c>
       <c r="E5" t="n">
-        <v>8922.911836624144</v>
+        <v>3196.02660369873</v>
       </c>
       <c r="F5" t="n">
-        <v>8783.810222625731</v>
+        <v>3141.488021850586</v>
       </c>
       <c r="G5" t="n">
-        <v>7828.138624191283</v>
+        <v>2804.028327941895</v>
       </c>
       <c r="H5" t="n">
-        <v>8102.020219802856</v>
+        <v>2897.524291992188</v>
       </c>
       <c r="I5" t="n">
-        <v>7968.988214492797</v>
+        <v>2853.952606201172</v>
       </c>
       <c r="J5" t="n">
-        <v>8389.879205703737</v>
+        <v>2979.644393920898</v>
       </c>
       <c r="K5" t="n">
-        <v>8337.542638778687</v>
+        <v>2966.086006164551</v>
       </c>
       <c r="L5" t="n">
-        <v>9033.397521972656</v>
+        <v>3431.16396484375</v>
       </c>
       <c r="M5" t="n">
-        <v>8987.148376464844</v>
+        <v>3411.730419921875</v>
       </c>
     </row>
   </sheetData>
@@ -1639,40 +1640,40 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>2869.994298240451</v>
+        <v>3310.166880611683</v>
       </c>
       <c r="C2" t="n">
-        <v>4325.699175203388</v>
+        <v>4566.885454637843</v>
       </c>
       <c r="D2" t="n">
-        <v>3403.86203508394</v>
+        <v>4035.894295328839</v>
       </c>
       <c r="E2" t="n">
-        <v>5194.683909093721</v>
+        <v>6082.349859288737</v>
       </c>
       <c r="F2" t="n">
-        <v>5890.802407626777</v>
+        <v>6896.087144142321</v>
       </c>
       <c r="G2" t="n">
-        <v>10452.86691380985</v>
+        <v>12246.73775012768</v>
       </c>
       <c r="H2" t="n">
-        <v>15401.27092554241</v>
+        <v>15892.24487152819</v>
       </c>
       <c r="I2" t="n">
-        <v>20305.46494609306</v>
+        <v>20826.87735016263</v>
       </c>
       <c r="J2" t="n">
-        <v>24856.90141717593</v>
+        <v>23066.53065781126</v>
       </c>
       <c r="K2" t="n">
-        <v>28169.88832810346</v>
+        <v>25995.69952495382</v>
       </c>
       <c r="L2" t="n">
-        <v>26749.8830608565</v>
+        <v>24908.89831026768</v>
       </c>
       <c r="M2" t="n">
-        <v>30167.84688158268</v>
+        <v>28053.23879859319</v>
       </c>
     </row>
     <row r="3">
@@ -1682,40 +1683,40 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0.72088</v>
+        <v>0.72036</v>
       </c>
       <c r="C3" t="n">
-        <v>0.44358</v>
+        <v>0.52918</v>
       </c>
       <c r="D3" t="n">
-        <v>0.7206399999999999</v>
+        <v>0.72044</v>
       </c>
       <c r="E3" t="n">
-        <v>0.4436</v>
+        <v>0.44298</v>
       </c>
       <c r="F3" t="n">
-        <v>0.38456</v>
+        <v>0.38364</v>
       </c>
       <c r="G3" t="n">
-        <v>0.1923</v>
+        <v>0.19182</v>
       </c>
       <c r="H3" t="n">
-        <v>0.12802</v>
+        <v>0.15272</v>
       </c>
       <c r="I3" t="n">
-        <v>0.09616</v>
+        <v>0.11452</v>
       </c>
       <c r="J3" t="n">
-        <v>0.07679999999999999</v>
+        <v>0.10908</v>
       </c>
       <c r="K3" t="n">
-        <v>0.068</v>
+        <v>0.09618</v>
       </c>
       <c r="L3" t="n">
-        <v>0.07702000000000001</v>
+        <v>0.10878</v>
       </c>
       <c r="M3" t="n">
-        <v>0.06802</v>
+        <v>0.09601999999999999</v>
       </c>
     </row>
     <row r="4">
@@ -1726,62 +1727,62 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>(5122.22, 5843.1)</t>
+          <t>(4781.74, 5502.1)</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>(8604.7, 9048.28)</t>
+          <t>(8994.72, 9523.9)</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>(12731.98, 13452.62)</t>
+          <t>(13748.18, 14468.62)</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>(16026.24, 16469.84)</t>
+          <t>(17856.92, 18299.9)</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>(18804.3, 19188.86)</t>
+          <t>(21174.44, 21558.08)</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>(20754.8, 20947.1)</t>
+          <t>(23605.3, 23797.12)</t>
         </is>
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>(22310.1, 22438.12)</t>
+          <t>(25424.88, 25577.6)</t>
         </is>
       </c>
       <c r="I4" t="inlineStr">
         <is>
-          <t>(23660.04, 23756.2)</t>
+          <t>(27006.36, 27120.88)</t>
         </is>
       </c>
       <c r="J4" t="inlineStr">
         <is>
-          <t>(24923.44, 25000.24)</t>
+          <t>(28447.86, 28556.94)</t>
         </is>
       </c>
       <c r="K4" t="inlineStr">
         <is>
-          <t>(26123.54, 26191.54)</t>
+          <t>(29826.5, 29922.68)</t>
         </is>
       </c>
       <c r="L4" t="inlineStr">
         <is>
-          <t>(27357.38, 27434.4)</t>
+          <t>(31222.98, 31331.76)</t>
         </is>
       </c>
       <c r="M4" t="inlineStr">
         <is>
-          <t>(28557.46, 28625.48)</t>
+          <t>(32600.88, 32696.9)</t>
         </is>
       </c>
     </row>
@@ -1792,40 +1793,317 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>6827.440916061401</v>
+        <v>2384.511814117432</v>
       </c>
       <c r="C5" t="n">
-        <v>6332.019012451171</v>
+        <v>2416.704444885254</v>
       </c>
       <c r="D5" t="n">
-        <v>8094.765151977538</v>
+        <v>3489.143623352051</v>
       </c>
       <c r="E5" t="n">
-        <v>7604.393880844115</v>
+        <v>3233.23120880127</v>
       </c>
       <c r="F5" t="n">
-        <v>7475.711013793945</v>
+        <v>3174.737846374511</v>
       </c>
       <c r="G5" t="n">
-        <v>6633.284814834595</v>
+        <v>2819.00308227539</v>
       </c>
       <c r="H5" t="n">
-        <v>6506.513322830199</v>
+        <v>2912.476364135742</v>
       </c>
       <c r="I5" t="n">
-        <v>6443.492580413817</v>
+        <v>2862.11279296875</v>
       </c>
       <c r="J5" t="n">
-        <v>6299.733095169066</v>
+        <v>3019.316596984863</v>
       </c>
       <c r="K5" t="n">
-        <v>6321.322940826416</v>
+        <v>3000.31965637207</v>
       </c>
       <c r="L5" t="n">
-        <v>6798.910778045654</v>
+        <v>3468.275146484375</v>
       </c>
       <c r="M5" t="n">
-        <v>6771.655918121337</v>
+        <v>3447.900146484375</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:M5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="B1" s="2" t="inlineStr">
+        <is>
+          <t>16_RANGE2</t>
+        </is>
+      </c>
+      <c r="C1" s="2" t="inlineStr">
+        <is>
+          <t>26_RANGE2</t>
+        </is>
+      </c>
+      <c r="D1" s="2" t="inlineStr">
+        <is>
+          <t>16</t>
+        </is>
+      </c>
+      <c r="E1" s="2" t="inlineStr">
+        <is>
+          <t>26</t>
+        </is>
+      </c>
+      <c r="F1" s="2" t="inlineStr">
+        <is>
+          <t>30</t>
+        </is>
+      </c>
+      <c r="G1" s="2" t="inlineStr">
+        <is>
+          <t>60</t>
+        </is>
+      </c>
+      <c r="H1" s="2" t="inlineStr">
+        <is>
+          <t>90</t>
+        </is>
+      </c>
+      <c r="I1" s="2" t="inlineStr">
+        <is>
+          <t>120</t>
+        </is>
+      </c>
+      <c r="J1" s="2" t="inlineStr">
+        <is>
+          <t>150</t>
+        </is>
+      </c>
+      <c r="K1" s="2" t="inlineStr">
+        <is>
+          <t>170</t>
+        </is>
+      </c>
+      <c r="L1" s="2" t="inlineStr">
+        <is>
+          <t>150_BOOST</t>
+        </is>
+      </c>
+      <c r="M1" s="2" t="inlineStr">
+        <is>
+          <t>170_BOOST</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="2" t="inlineStr">
+        <is>
+          <t>intensity</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>2854.467398643865</v>
+      </c>
+      <c r="C2" t="n">
+        <v>4298.727748465543</v>
+      </c>
+      <c r="D2" t="n">
+        <v>3411.518237102271</v>
+      </c>
+      <c r="E2" t="n">
+        <v>5139.659541688737</v>
+      </c>
+      <c r="F2" t="n">
+        <v>5849.352104026038</v>
+      </c>
+      <c r="G2" t="n">
+        <v>10346.92391394675</v>
+      </c>
+      <c r="H2" t="n">
+        <v>15205.82588667575</v>
+      </c>
+      <c r="I2" t="n">
+        <v>19937.52837181091</v>
+      </c>
+      <c r="J2" t="n">
+        <v>24741.13283695853</v>
+      </c>
+      <c r="K2" t="n">
+        <v>27828.084808035</v>
+      </c>
+      <c r="L2" t="n">
+        <v>26577.64379226879</v>
+      </c>
+      <c r="M2" t="n">
+        <v>29907.02812628798</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="2" t="inlineStr">
+        <is>
+          <t>runtime</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>0.71996</v>
+      </c>
+      <c r="C3" t="n">
+        <v>0.4433</v>
+      </c>
+      <c r="D3" t="n">
+        <v>0.72006</v>
+      </c>
+      <c r="E3" t="n">
+        <v>0.44308</v>
+      </c>
+      <c r="F3" t="n">
+        <v>0.3839</v>
+      </c>
+      <c r="G3" t="n">
+        <v>0.19202</v>
+      </c>
+      <c r="H3" t="n">
+        <v>0.12808</v>
+      </c>
+      <c r="I3" t="n">
+        <v>0.096</v>
+      </c>
+      <c r="J3" t="n">
+        <v>0.07686</v>
+      </c>
+      <c r="K3" t="n">
+        <v>0.0679</v>
+      </c>
+      <c r="L3" t="n">
+        <v>0.07686</v>
+      </c>
+      <c r="M3" t="n">
+        <v>0.06786</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="2" t="inlineStr">
+        <is>
+          <t>timestamp</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>(5601.84, 6321.8)</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>(9623.48, 10066.78)</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>(14567.96, 15288.02)</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>(18399.08, 18842.16)</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>(21657.56, 22041.46)</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>(23896.5, 24088.52)</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>(25677.0, 25805.08)</t>
+        </is>
+      </c>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>(27220.2, 27316.2)</t>
+        </is>
+      </c>
+      <c r="J4" t="inlineStr">
+        <is>
+          <t>(28656.16, 28733.02)</t>
+        </is>
+      </c>
+      <c r="K4" t="inlineStr">
+        <is>
+          <t>(30022.02, 30089.92)</t>
+        </is>
+      </c>
+      <c r="L4" t="inlineStr">
+        <is>
+          <t>(31430.84, 31507.7)</t>
+        </is>
+      </c>
+      <c r="M4" t="inlineStr">
+        <is>
+          <t>(32796.04, 32863.9)</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="2" t="inlineStr">
+        <is>
+          <t>energy</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>2055.102348327637</v>
+      </c>
+      <c r="C5" t="n">
+        <v>1905.626010894775</v>
+      </c>
+      <c r="D5" t="n">
+        <v>2947.797386169434</v>
+      </c>
+      <c r="E5" t="n">
+        <v>2732.736419677734</v>
+      </c>
+      <c r="F5" t="n">
+        <v>2694.679527282715</v>
+      </c>
+      <c r="G5" t="n">
+        <v>2384.179595947265</v>
+      </c>
+      <c r="H5" t="n">
+        <v>2337.074615478516</v>
+      </c>
+      <c r="I5" t="n">
+        <v>2296.803268432617</v>
+      </c>
+      <c r="J5" t="n">
+        <v>2281.924163818359</v>
+      </c>
+      <c r="K5" t="n">
+        <v>2267.432350158691</v>
+      </c>
+      <c r="L5" t="n">
+        <v>2614.729858398438</v>
+      </c>
+      <c r="M5" t="n">
+        <v>2597.748388671875</v>
       </c>
     </row>
   </sheetData>

</xml_diff>